<commit_message>
added homework to the 1st and the 2nd seminars
</commit_message>
<xml_diff>
--- a/Seminar1/семинар1.xlsx
+++ b/Seminar1/семинар1.xlsx
@@ -2,21 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AyDaR\Downloads\фин матматик\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Елена\Desktop\Geekbrains\Финансовая математика\Seminar1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" firstSheet="11" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" firstSheet="7" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
     <sheet name="Лист4" sheetId="4" r:id="rId4"/>
-    <sheet name="Лист4 (2)" sheetId="5" r:id="rId5"/>
+    <sheet name="Лист5" sheetId="5" r:id="rId5"/>
     <sheet name="Лист6" sheetId="6" r:id="rId6"/>
     <sheet name="Лист7" sheetId="7" r:id="rId7"/>
     <sheet name="Лист8" sheetId="8" r:id="rId8"/>
@@ -32,8 +32,9 @@
     <sheet name="Лист18" sheetId="18" r:id="rId18"/>
     <sheet name="Лист19" sheetId="19" r:id="rId19"/>
     <sheet name="Лист20" sheetId="20" r:id="rId20"/>
+    <sheet name="Лист21" sheetId="21" r:id="rId21"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="92">
   <si>
     <t>Срок</t>
   </si>
@@ -110,17 +111,228 @@
   <si>
     <t>инфляция</t>
   </si>
+  <si>
+    <t>Банк предлагает два варианта размещения депозита в размере 1 млн руб. на 3 года: либо под 15% годовых по схеме сложных процентов (с капитализацией),</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> либо под 20% годовых по схеме простых процентов. Какой вариант выгоднее для заемщика?</t>
+  </si>
+  <si>
+    <t>ставка</t>
+  </si>
+  <si>
+    <t>итого через 3 года</t>
+  </si>
+  <si>
+    <t>Инвестор хочет через 25 лет выйти на пенсию и купить домик в Испании. Он планирует, что для этого нужно будет иметь €350 тыс.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Если текущая доходность банковского депозита в Европе равна 3% годовых, то сколько нужно положить в банк сейчас, чтобы через 25 лет получить нужную сумму?</t>
+  </si>
+  <si>
+    <t>вклад</t>
+  </si>
+  <si>
+    <t>итого чере 25 лет</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Банк предлагает положить депозит 3 млн руб. на 6 лет, обещая выплатить 1,5 млн руб. процентов в конце срока. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Какую процентную ставку предлагает банк, если подразумевается начисление процентов раз в год по сложной ставке? </t>
+  </si>
+  <si>
+    <t>Итого через 6 лет</t>
+  </si>
+  <si>
+    <t>Ставка</t>
+  </si>
+  <si>
+    <t>Депозит</t>
+  </si>
+  <si>
+    <t>Клиент банка взял кредит в размере 150 тыс.руб. на 2 года под 14% годовых с ежегодным начислением процентов и возвратом кредита и всех накопленных процентов в конце срока.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Определить величину переплаты по кредиту по сравнению с изначальной суммой</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Клиент банка взял кредит в размере 150 тыс.руб. на 2 года под 14% годовых с ежемесячным начислением процентов и возвратом кредита и всех накопленных процентов в конце срока. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Определить величину переплаты по кредиту по сравнению с изначальной суммой. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Вкладчик внес в банк некую сумму денег под 12% годовых с начислением сложных процентов раз в квартал. </t>
+  </si>
+  <si>
+    <t>Через 7 лет на счету у него оказалось 30 млн.руб. Какую сумму положил в банк вкладчик?</t>
+  </si>
+  <si>
+    <t>Какая доходность должна быть у инвестиций, чтобы они позволили инвестору увеличить свои вложения в 2 раза на горизонте 5 лет?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Менеджер получил годовой бонус в размере 2,5 млн руб. и хочет отдать его в управление профессиональному трейдеру на фондовом рынке. </t>
+  </si>
+  <si>
+    <t>Какую сумму он может ожидать получить через 15 лет, если средняя доходность, которую ему обещает трейдер, составит 12% годовых?</t>
+  </si>
+  <si>
+    <t>Микрофинансовая организация начисляет 0.5% за каждый день пользования кредитом (исходя из 365 дней в году). Какая эффективная ставка по этому кредиту?</t>
+  </si>
+  <si>
+    <t>Инвестор подвел итоги года и рассчитал, что за год его инвестиции принесли доходность 18%.</t>
+  </si>
+  <si>
+    <t>Если инфляция в стране за этот период составила 7%, какая реальная доходность его инвестиций?</t>
+  </si>
+  <si>
+    <t>Если в договоре банковского депозита предусмотрено ежеквартальное начисление процентов по номинальной ставке 10% годовых, то какова эффективная ставка?</t>
+  </si>
+  <si>
+    <t>Эффективная ставка</t>
+  </si>
+  <si>
+    <t>Ном.ставка</t>
+  </si>
+  <si>
+    <t>Периодичность начислений</t>
+  </si>
+  <si>
+    <t>Инвестционный фонд сообщил своим участникам, что номинальная доходность инвестиций составила 12% за год, в то время как реальная – только 8,5%. Какая инфляция была заложена в расчеты?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Согласно договору со страховой компанией по договору накопительной пенсии она гарантирует выплаты в размере 250 тыс. руб./год в течение 15 лет. </t>
+  </si>
+  <si>
+    <t>Если стоимость денег равна 10% годовых, то сколько будет стоить такой пенсионный контракт сейчас?</t>
+  </si>
+  <si>
+    <t>выплата</t>
+  </si>
+  <si>
+    <t>стоимость денег</t>
+  </si>
+  <si>
+    <t>цена контракта</t>
+  </si>
+  <si>
+    <t>Если класть в банк по $100 ежемесячно в течение 10 лет, начиная со следующего месяца, а банк при этом начисляет 8% годовых, то какая сумма получится на депозите через 20 лет?</t>
+  </si>
+  <si>
+    <t>депозит</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ставка </t>
+  </si>
+  <si>
+    <t>итого через 20 лет</t>
+  </si>
+  <si>
+    <t>срок вкладов</t>
+  </si>
+  <si>
+    <t>срок депозита</t>
+  </si>
+  <si>
+    <t>итого через 10 лет</t>
+  </si>
+  <si>
+    <t>Если в предыдущей задаче срок такой ренты в договоре  будет бесконечным (то есть, юридически до момента смерти пенсионера), то каков размер ежемесячного платежа?</t>
+  </si>
+  <si>
+    <t>договор</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Для обеспечения себя будущей пенсией человек заключил договор финансовой ренты на 20 лет по ставке 12% годовых. В момент заключения он заплатил 7 млн руб. </t>
+  </si>
+  <si>
+    <t>Оплата ренты будет проходить в виде ежемесячных аннуитетных платежей. Какой будет размер этого платежа?</t>
+  </si>
+  <si>
+    <t>ежемес. выплата</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Есть 3-х летняя облигация, номиналом $1000 и купоном 5%, уплачиваемым 1 раз в год. </t>
+  </si>
+  <si>
+    <t>Текущая цена равна $900. Какова доходность этой облигации?</t>
+  </si>
+  <si>
+    <t>номинал</t>
+  </si>
+  <si>
+    <t>купон</t>
+  </si>
+  <si>
+    <t>цена</t>
+  </si>
+  <si>
+    <t>доходность</t>
+  </si>
+  <si>
+    <t>Каков номинал 4-х летней облигации, если ее рыночная цена = 1100 руб., по ней платится ежегодный купон в размере 100 руб., и ее доходность равна 12% годовых.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Есть 7-ми летняя облигация, номиналом 1 000 руб. и с купоном 12%, уплачиваемым 2 раза в год. </t>
+  </si>
+  <si>
+    <t>Пусть стоимость денег для держателя облигации равна 10% годовых. Какова справедливая цена облигации?</t>
+  </si>
+  <si>
+    <t>справедливая цена</t>
+  </si>
+  <si>
+    <t>выплаты по купону</t>
+  </si>
+  <si>
+    <t>Рыночная цена облигации равна 950 руб. Какова доходность облигации (т.е. стоимость денег)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Заемщик получил в банке кредит размером 1 млн руб., выданный на 2 года под ставку 16% годовых, с ежемесячными аннуитетными платежами. </t>
+  </si>
+  <si>
+    <t>Определить размер совокупной переплаты для заемщика.</t>
+  </si>
+  <si>
+    <t>кредит</t>
+  </si>
+  <si>
+    <t>платеж за мес</t>
+  </si>
+  <si>
+    <t>платеж за 2 года</t>
+  </si>
+  <si>
+    <t>лизинг</t>
+  </si>
+  <si>
+    <t>погашения</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Банк предлагает два варианта финансирования 3 млн.руб.: </t>
+  </si>
+  <si>
+    <t>либо кредит под 10% годовых на 4 года с ежеквартальным погашением,Определить, какой вариант выгодней с точки зрения переплаты</t>
+  </si>
+  <si>
+    <t>выкуп.сумма</t>
+  </si>
+  <si>
+    <t xml:space="preserve">либо лизинг под 11% годовых на 3 года с ежемесячным аннуитетным погашением и выкупной суммой 500 тыс.руб. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
-    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;₸&quot;;[Red]\-#,##0.00\ &quot;₸&quot;"/>
-    <numFmt numFmtId="166" formatCode="0.000%"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="4">
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;₽&quot;;[Red]\-#,##0.00\ &quot;₽&quot;"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,16 +341,39 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -146,22 +381,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Финансовый" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -439,75 +705,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="C2" s="5">
+        <f>A2*(1+B2)^A3</f>
+        <v>1520874.9999999995</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="C3" s="6">
+        <f>A2*(1+B3*A3)</f>
+        <v>1600000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1000000</v>
-      </c>
-      <c r="C1">
-        <v>0.15</v>
-      </c>
-      <c r="E1">
-        <f>A1*(1+C1)^A2</f>
-        <v>1520874.9999999995</v>
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>0.2</v>
-      </c>
-      <c r="E2">
-        <f>A1*(1+C2*A2)</f>
-        <v>1600000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="8">
         <v>0.18</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="8">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="7">
         <f>(1+A2)/(1+B2)-1</f>
         <v>0.10280373831775691</v>
       </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -516,14 +807,40 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>4</v>
+      </c>
+      <c r="C2" s="7">
         <f>(1+10%/4)^4-1</f>
         <v>0.10381289062499977</v>
       </c>
@@ -537,32 +854,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="C1" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="8">
         <v>0.12</v>
       </c>
-      <c r="C2" s="1">
+      <c r="B2" s="7">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="E2" s="1">
-        <f>(1+A2)/(1+C2)-1</f>
+      <c r="C2" s="7">
+        <f>(1+A2)/(1+B2)-1</f>
         <v>3.2258064516129226E-2</v>
       </c>
     </row>
@@ -573,20 +893,52 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>250000</v>
+      </c>
+      <c r="C2" s="2">
+        <v>15</v>
+      </c>
+      <c r="D2" s="9">
         <f>PV(10%,15,-250)</f>
         <v>1901.5198765770915</v>
       </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -595,25 +947,59 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>100</v>
+      </c>
+      <c r="B2" s="2">
+        <v>10</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="D2" s="2">
+        <v>20</v>
+      </c>
+      <c r="E2" s="9">
         <f>FV(8%/12,10*12,-100)</f>
         <v>18294.603518170716</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="F2" s="9">
         <f>FV(8%/12,10*12,0,-18294.6)</f>
         <v>40607.430234901731</v>
       </c>
@@ -625,20 +1011,70 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>7000000</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="C2" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="10">
         <f>PMT(12%/12,12*20,-7000000)</f>
         <v>77076.029349872697</v>
       </c>
+      <c r="F2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
+        <f>A2*B2/12</f>
+        <v>70000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -647,17 +1083,57 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>900</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3</v>
+      </c>
+      <c r="E2" s="11">
         <f>RATE(3,5%*1000,-900,1000)</f>
         <v>8.9468026327162928E-2</v>
       </c>
+      <c r="G2" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -666,17 +1142,51 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1100</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="C2" s="2">
+        <v>100</v>
+      </c>
+      <c r="D2" s="2">
+        <v>4</v>
+      </c>
+      <c r="E2" s="12">
         <f>FV(12%,4,100,-1100)</f>
         <v>1252.9384960000002</v>
       </c>
@@ -688,20 +1198,60 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="E2" s="13">
         <f>-PV(10%/2,2*7,12%*1000/2,1000)</f>
         <v>1098.9864094008963</v>
       </c>
+      <c r="G2" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -710,47 +1260,107 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>950</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>7</v>
+      </c>
+      <c r="F2" s="8">
+        <f>RATE(14,12%*1000/2,-950,1000)</f>
+        <v>6.5566177421156988E-2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2">
-        <f>RATE(14,12%*1000/2,-950,1000)</f>
-        <v>6.5566177421156988E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <f>C2/(1+B2)^25</f>
+        <v>167161.94924158088</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="C2" s="2">
         <v>350000</v>
       </c>
-      <c r="B1">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f>A1/(1+B1)^25</f>
-        <v>167161.94924158088</v>
+      <c r="E2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -760,74 +1370,211 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A18"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="12">
         <f>PMT(16%/12,24,-1000000)</f>
         <v>48963.110517610046</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <f>A1*24</f>
+      <c r="E2" s="2">
+        <f>D2*24</f>
         <v>1175114.6524226412</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f>A2-1000000</f>
+      <c r="F2" s="2">
+        <f>E2-1000000</f>
         <v>175114.65242264117</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="H2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="14"/>
+      <c r="F1" s="15">
         <f>PMT(10%/4,4*4,-3000000)</f>
         <v>229796.96581795407</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f>A11*4*4</f>
+      <c r="H1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>3000000</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2">
+        <f>F1*4*4</f>
         <v>3676751.4530872651</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f>A12-3000000</f>
+      <c r="H2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2">
+        <f>F2-3000000</f>
         <v>676751.45308726514</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="H3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3000000</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2">
+        <v>500000</v>
+      </c>
+      <c r="F5" s="10">
         <f>PMT(11%/12,12*3,-3000000,500000)</f>
         <v>86430.126125838447</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f>A15*12*3</f>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2">
+        <f>F5*12*3</f>
         <v>3111484.5405301843</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f>A16+500000</f>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2">
+        <f>F6+500000</f>
         <v>3611484.5405301843</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f>A17-3000000</f>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="4">
+        <f>F7-3000000</f>
         <v>611484.54053018428</v>
       </c>
     </row>
@@ -838,37 +1585,57 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>3</v>
       </c>
-      <c r="B1">
+      <c r="B2" s="7">
+        <f>B3-1</f>
+        <v>6.991319393366302E-2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2">
         <v>4.5</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f>(B1/A1)^(1/E1)</f>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2">
+        <f>(D2/A2)^(1/C2)</f>
         <v>1.069913193933663</v>
       </c>
-      <c r="B4" s="1">
-        <f>A4-1</f>
-        <v>6.991319393366302E-2</v>
-      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -877,49 +1644,55 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>150000</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <f>A2*(1+B2)^C2</f>
         <v>194940.00000000006</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <f>D2-A2</f>
         <v>44940.000000000058</v>
       </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -928,10 +1701,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,40 +1712,46 @@
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="G1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>150000</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>12</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <f>A2*(1+B2/D2)^(C2*D2)</f>
         <v>198148.06501530399</v>
       </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -981,48 +1760,54 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>30</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="8">
         <v>0.12</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>4</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>7</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <f>A2/(1+B2/C2)^(D2*C2)</f>
         <v>13.112302595112768</v>
       </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1031,25 +1816,30 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A5"/>
-  <sheetViews>
-    <sheetView zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f>2^(1/5)-1</f>
         <v>0.1486983549970351</v>
@@ -1062,42 +1852,48 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>2.5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>15</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="8">
         <v>0.12</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <f>A2*(1+C2)^B2</f>
         <v>13.683914398142607</v>
       </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1106,15 +1902,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>(1+0.005)^365</f>
         <v>6.1746527834309033</v>
@@ -1123,6 +1919,9 @@
         <f>A1-1</f>
         <v>5.1746527834309033</v>
       </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>